<commit_message>
Power point presentation added
</commit_message>
<xml_diff>
--- a/All_Stats.xlsx
+++ b/All_Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tesi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldob\Documents\GitHub\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669B66D8-8776-4AB9-A154-D977707B1756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8659DE-47AA-41D0-88A8-5A26BDEF2A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{EBFCFC75-FC7A-4F61-9347-6E3644117AA3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{EBFCFC75-FC7A-4F61-9347-6E3644117AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="542">
   <si>
     <t>Episode1</t>
   </si>
@@ -1605,6 +1605,60 @@
   </si>
   <si>
     <t>0.1379</t>
+  </si>
+  <si>
+    <t>Without BUK class</t>
+  </si>
+  <si>
+    <t>With BUK class</t>
+  </si>
+  <si>
+    <t>Mean Class F1_score: 0.5612</t>
+  </si>
+  <si>
+    <t>Mean f1_score=0.3108</t>
+  </si>
+  <si>
+    <t>Mean precision=0.31175</t>
+  </si>
+  <si>
+    <t>Mean recall= 0.3501</t>
+  </si>
+  <si>
+    <t>Mean Class. F1_score:0.5617</t>
+  </si>
+  <si>
+    <t>Mean f1_score=0.3621</t>
+  </si>
+  <si>
+    <t>Mean precision=0.3469</t>
+  </si>
+  <si>
+    <t>Mean recall= 0.4194</t>
+  </si>
+  <si>
+    <t>Mean Class. F1_score:0.5451</t>
+  </si>
+  <si>
+    <t>Mean f1_score=0.3784</t>
+  </si>
+  <si>
+    <t>Mean precision=0.697</t>
+  </si>
+  <si>
+    <t>Mean recall= 0.373</t>
+  </si>
+  <si>
+    <t>Mean Class. F1_score:0.5270</t>
+  </si>
+  <si>
+    <t>Mean f1_score=0.3364</t>
+  </si>
+  <si>
+    <t>Mean precision=0.433</t>
+  </si>
+  <si>
+    <t>Mean recall= 0.3531</t>
   </si>
 </sst>
 </file>
@@ -1678,18 +1732,7 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4834,10 +4877,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76DD7574-9F37-4FBA-838D-B915853182C8}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4847,9 +4890,10 @@
     <col min="3" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="4" width="20.21875" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>178</v>
       </c>
@@ -4865,28 +4909,46 @@
       <c r="E1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" t="s">
+        <v>526</v>
+      </c>
+      <c r="C2" t="s">
+        <v>527</v>
+      </c>
+      <c r="D2" t="s">
+        <v>528</v>
+      </c>
+      <c r="E2" t="s">
+        <v>529</v>
+      </c>
+      <c r="G2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>389</v>
       </c>
@@ -4900,7 +4962,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -4917,7 +4979,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -4934,7 +4996,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
@@ -4951,7 +5013,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>393</v>
       </c>
@@ -4968,7 +5030,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -4985,7 +5047,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>394</v>
       </c>
@@ -5002,7 +5064,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>395</v>
       </c>
@@ -5019,7 +5081,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>396</v>
       </c>
@@ -5036,7 +5098,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>397</v>
       </c>
@@ -5053,7 +5115,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>398</v>
       </c>
@@ -5213,10 +5275,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C287710-4B54-427C-88BF-DCF720751293}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5226,9 +5288,10 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="22.77734375" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>178</v>
       </c>
@@ -5244,28 +5307,46 @@
       <c r="E1" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="H1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:8">
       <c r="B7" t="s">
         <v>389</v>
       </c>
@@ -5279,7 +5360,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>75</v>
       </c>
@@ -5296,7 +5377,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>76</v>
       </c>
@@ -5313,7 +5394,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>77</v>
       </c>
@@ -5330,7 +5411,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>393</v>
       </c>
@@ -5347,7 +5428,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>79</v>
       </c>
@@ -5364,7 +5445,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>394</v>
       </c>
@@ -5381,7 +5462,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>395</v>
       </c>
@@ -5398,7 +5479,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>396</v>
       </c>
@@ -5415,7 +5496,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>397</v>
       </c>
@@ -5592,10 +5673,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DC4C3C-56A7-4487-B49D-5FD0A5C135B0}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C23"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5605,9 +5686,10 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="22.77734375" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>174</v>
       </c>
@@ -5623,23 +5705,41 @@
       <c r="E1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="H1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C2" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2" t="s">
+        <v>536</v>
+      </c>
+      <c r="E2" t="s">
+        <v>537</v>
+      </c>
+      <c r="H2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:8">
       <c r="B6" t="s">
         <v>389</v>
       </c>
@@ -5653,7 +5753,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -5670,7 +5770,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -5687,7 +5787,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
@@ -5704,7 +5804,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>393</v>
       </c>
@@ -5721,7 +5821,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>394</v>
       </c>
@@ -5738,7 +5838,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>395</v>
       </c>
@@ -5755,7 +5855,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>396</v>
       </c>
@@ -5772,7 +5872,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>397</v>
       </c>
@@ -5789,7 +5889,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>398</v>
       </c>
@@ -5806,7 +5906,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>399</v>
       </c>
@@ -5949,10 +6049,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6F0265-647B-4D78-A923-667BC941E242}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5962,9 +6062,10 @@
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="22.77734375" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>173</v>
       </c>
@@ -5980,23 +6081,41 @@
       <c r="E1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" t="s">
+        <v>538</v>
+      </c>
+      <c r="C2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E2" t="s">
+        <v>541</v>
+      </c>
+      <c r="G2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>389</v>
       </c>
@@ -6010,7 +6129,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -6027,7 +6146,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -6044,7 +6163,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
@@ -6061,7 +6180,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>393</v>
       </c>
@@ -6078,7 +6197,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
@@ -6095,7 +6214,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>394</v>
       </c>
@@ -6112,7 +6231,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>395</v>
       </c>
@@ -6129,7 +6248,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>396</v>
       </c>
@@ -6146,7 +6265,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>397</v>
       </c>
@@ -6163,7 +6282,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>398</v>
       </c>

</xml_diff>